<commit_message>
Add missing Format methods
</commit_message>
<xml_diff>
--- a/test/expected/format_border.xlsx
+++ b/test/expected/format_border.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>AAA</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>DDD</t>
+  </si>
+  <si>
+    <t>EEE</t>
   </si>
 </sst>
 </file>
@@ -49,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -101,16 +104,26 @@
         <color rgb="FFFF0000"/>
       </diagonal>
     </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thick">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,13 +418,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,6 +437,9 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>